<commit_message>
Primary, Secondary, and High School Data Cleaned
</commit_message>
<xml_diff>
--- a/Datasets/Ciudades_y_sus_Areas_Metropolitanas_en_GEIH.xlsx
+++ b/Datasets/Ciudades_y_sus_Areas_Metropolitanas_en_GEIH.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dda39ef004021ca5/Documents/GitHub/Hertie_School_MDS_Master_Thesis/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="14_{F4D8BE8C-9D96-4DB3-AF9B-F7AA3873154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA2E3BE6-F84D-40C4-B058-BE6DB362BA09}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="14_{F4D8BE8C-9D96-4DB3-AF9B-F7AA3873154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2680C159-42E0-476A-899A-7AB0C7A9B7B2}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-5520" windowWidth="29040" windowHeight="17520" xr2:uid="{294398BE-ACA2-4464-82F3-48684871EB93}"/>
+    <workbookView minimized="1" xWindow="6180" yWindow="3075" windowWidth="13500" windowHeight="8070" activeTab="1" xr2:uid="{294398BE-ACA2-4464-82F3-48684871EB93}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja2!$A$1:$G$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
   <si>
     <t>MEDELLÍN A.M.</t>
   </si>
@@ -258,6 +262,48 @@
   </si>
   <si>
     <t>cod_dane_mun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogotá D.C.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bucaramanga  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cartagena     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cúcuta        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ibagué       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medellín      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montería      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pasto         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pereira      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barranquilla  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Villavicencio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cali          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bogotá, D.C.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manizales     </t>
   </si>
 </sst>
 </file>
@@ -314,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -327,6 +373,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -664,8 +716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B63E3A4-6F38-4504-B0CF-6B0FFE33F22D}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,8 +755,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>29</v>
+      <c r="A2" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -719,61 +771,61 @@
         <v>48</v>
       </c>
       <c r="F2">
-        <v>8001</v>
+        <v>8758</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F3">
-        <v>8758</v>
+        <v>68307</v>
       </c>
       <c r="G3" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>31</v>
+      <c r="A4" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>49</v>
       </c>
       <c r="D4">
-        <v>11</v>
+        <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="F4">
-        <v>11001</v>
+        <v>68547</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
@@ -788,30 +840,30 @@
         <v>50</v>
       </c>
       <c r="F5">
-        <v>68001</v>
+        <v>68276</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F6">
-        <v>68307</v>
+        <v>76892</v>
       </c>
       <c r="G6" t="s">
         <v>67</v>
@@ -819,22 +871,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>49</v>
       </c>
       <c r="D7">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F7">
-        <v>68547</v>
+        <v>54874</v>
       </c>
       <c r="G7" t="s">
         <v>67</v>
@@ -842,22 +894,22 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>49</v>
       </c>
       <c r="D8">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F8">
-        <v>68276</v>
+        <v>54405</v>
       </c>
       <c r="G8" t="s">
         <v>67</v>
@@ -865,45 +917,45 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="D9">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="E9" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="F9">
-        <v>76001</v>
+        <v>91669</v>
       </c>
       <c r="G9" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F10">
-        <v>76892</v>
+        <v>54261</v>
       </c>
       <c r="G10" t="s">
         <v>67</v>
@@ -911,68 +963,68 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D11">
+        <v>17</v>
+      </c>
+      <c r="E11" t="s">
         <v>13</v>
       </c>
-      <c r="E11" t="s">
-        <v>53</v>
-      </c>
       <c r="F11">
-        <v>13001</v>
+        <v>17873</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D12">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F12">
-        <v>54001</v>
+        <v>5129</v>
       </c>
       <c r="G12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D13">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F13">
-        <v>54874</v>
+        <v>538</v>
       </c>
       <c r="G13" t="s">
         <v>67</v>
@@ -980,22 +1032,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D14">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F14">
-        <v>54405</v>
+        <v>5631</v>
       </c>
       <c r="G14" t="s">
         <v>67</v>
@@ -1003,22 +1055,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="F15">
-        <v>91669</v>
+        <v>536</v>
       </c>
       <c r="G15" t="s">
         <v>67</v>
@@ -1026,91 +1078,91 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D16">
-        <v>54</v>
+        <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F16">
-        <v>54261</v>
+        <v>5266</v>
       </c>
       <c r="G16" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
+      <c r="A17" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D17">
-        <v>73</v>
+        <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F17">
-        <v>73001</v>
+        <v>5088</v>
       </c>
       <c r="G17" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C18" t="s">
         <v>58</v>
       </c>
       <c r="D18">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F18">
-        <v>17001</v>
+        <v>5212</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>46</v>
+      <c r="A19" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C19" t="s">
         <v>58</v>
       </c>
       <c r="D19">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="F19">
-        <v>17873</v>
+        <v>5308</v>
       </c>
       <c r="G19" t="s">
         <v>67</v>
@@ -1118,7 +1170,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>0</v>
@@ -1133,53 +1185,53 @@
         <v>59</v>
       </c>
       <c r="F20">
-        <v>5001</v>
+        <v>5079</v>
       </c>
       <c r="G20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
         <v>58</v>
       </c>
       <c r="D21">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F21">
-        <v>5129</v>
+        <v>6617</v>
       </c>
       <c r="G21" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>39</v>
+      <c r="A22" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
         <v>58</v>
       </c>
       <c r="D22">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F22">
-        <v>538</v>
+        <v>664</v>
       </c>
       <c r="G22" t="s">
         <v>67</v>
@@ -1187,206 +1239,206 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="F23">
-        <v>5631</v>
+        <v>8001</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>41</v>
+      <c r="A24" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="F24">
-        <v>536</v>
+        <v>11001</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>42</v>
+      <c r="A25" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D25">
-        <v>5</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F25">
-        <v>5266</v>
+        <v>68001</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>76</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F26">
-        <v>5088</v>
+        <v>76001</v>
       </c>
       <c r="G26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D27">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F27">
-        <v>5212</v>
+        <v>13001</v>
       </c>
       <c r="G27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F28">
-        <v>5308</v>
+        <v>54001</v>
       </c>
       <c r="G28" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>73</v>
+      </c>
+      <c r="E29" t="s">
+        <v>57</v>
+      </c>
+      <c r="F29">
+        <v>73001</v>
+      </c>
+      <c r="G29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
         <v>58</v>
       </c>
-      <c r="D29">
-        <v>5</v>
-      </c>
-      <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="F29">
-        <v>5079</v>
-      </c>
-      <c r="G29" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
       <c r="D30">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
-        <v>60</v>
+        <v>13</v>
       </c>
       <c r="F30">
-        <v>23001</v>
+        <v>17001</v>
       </c>
       <c r="G30" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>35</v>
+      <c r="A31" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="D31">
-        <v>52</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F31">
-        <v>52001</v>
+        <v>5001</v>
       </c>
       <c r="G31" t="s">
         <v>66</v>
@@ -1394,22 +1446,22 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D32">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="E32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F32">
-        <v>66001</v>
+        <v>23001</v>
       </c>
       <c r="G32" t="s">
         <v>66</v>
@@ -1417,30 +1469,30 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D33">
+        <v>52</v>
+      </c>
+      <c r="E33" t="s">
+        <v>61</v>
+      </c>
+      <c r="F33">
+        <v>52001</v>
+      </c>
+      <c r="G33" t="s">
         <v>66</v>
-      </c>
-      <c r="E33" t="s">
-        <v>62</v>
-      </c>
-      <c r="F33">
-        <v>6617</v>
-      </c>
-      <c r="G33" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>9</v>
@@ -1455,10 +1507,10 @@
         <v>62</v>
       </c>
       <c r="F34">
-        <v>664</v>
+        <v>66001</v>
       </c>
       <c r="G34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1482,6 +1534,142 @@
       </c>
       <c r="G35" t="s">
         <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{7B63E3A4-6F38-4504-B0CF-6B0FFE33F22D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G35">
+      <sortCondition ref="G1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7251F6B-8B3E-4325-A111-004E099EF1D2}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cleaning Poverty Data Set and Gathering More for cleaning
</commit_message>
<xml_diff>
--- a/Datasets/Ciudades_y_sus_Areas_Metropolitanas_en_GEIH.xlsx
+++ b/Datasets/Ciudades_y_sus_Areas_Metropolitanas_en_GEIH.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dda39ef004021ca5/Documents/GitHub/Hertie_School_MDS_Master_Thesis/Datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="87" documentId="14_{F4D8BE8C-9D96-4DB3-AF9B-F7AA3873154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2680C159-42E0-476A-899A-7AB0C7A9B7B2}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="14_{F4D8BE8C-9D96-4DB3-AF9B-F7AA3873154B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{337D3A17-6342-441B-A743-F5B7852BFD1B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6180" yWindow="3075" windowWidth="13500" windowHeight="8070" activeTab="1" xr2:uid="{294398BE-ACA2-4464-82F3-48684871EB93}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{294398BE-ACA2-4464-82F3-48684871EB93}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="87">
   <si>
     <t>MEDELLÍN A.M.</t>
   </si>
@@ -292,9 +292,6 @@
   </si>
   <si>
     <t xml:space="preserve">Barranquilla  </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Villavicencio</t>
   </si>
   <si>
     <t xml:space="preserve">Cali          </t>
@@ -360,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -372,9 +369,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -716,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B63E3A4-6F38-4504-B0CF-6B0FFE33F22D}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +749,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -801,7 +795,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1100,7 +1094,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1146,7 +1140,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>45</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1215,7 +1209,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1284,7 +1278,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -1399,7 +1393,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -1422,7 +1416,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -1548,10 +1542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7251F6B-8B3E-4325-A111-004E099EF1D2}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B14"/>
+      <selection activeCell="F1" sqref="F1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,119 +1554,206 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>74</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>76</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>78</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>36</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F1:F14">
+    <sortCondition ref="F1:F14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>